<commit_message>
got rid of unecessary file
</commit_message>
<xml_diff>
--- a/TableResults.xlsx
+++ b/TableResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katya\OneDrive\Documents\ISE 3230 Project\ISE3230\ISE3230\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D90A32EE-CE7F-45BA-A975-03D9A4CAF892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB41A0CC-1434-4BCB-A821-0874F1D5D7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{965C898B-D708-433E-98F6-19A981446D10}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="4" activeTab="7" xr2:uid="{965C898B-D708-433E-98F6-19A981446D10}"/>
   </bookViews>
   <sheets>
     <sheet name="Tournaments 1-5" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,9 @@
     <sheet name="Tournaments 21-50" sheetId="3" r:id="rId3"/>
     <sheet name="Tournaments 51-100" sheetId="11" r:id="rId4"/>
     <sheet name="Tournaments 101-250" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet10" sheetId="10" r:id="rId6"/>
-    <sheet name="Tournaments 251-500" sheetId="6" r:id="rId7"/>
-    <sheet name="Tournaments 501-1000" sheetId="7" r:id="rId8"/>
-    <sheet name="Tournaments 1000+" sheetId="8" r:id="rId9"/>
+    <sheet name="Tournaments 251-500" sheetId="6" r:id="rId6"/>
+    <sheet name="Tournaments 501-1000" sheetId="7" r:id="rId7"/>
+    <sheet name="Tournaments 1000+" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -736,7 +735,7 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B1" sqref="B1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -933,7 +932,7 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A15"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1026,7 +1025,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1104,7 +1103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{040C05FE-5E00-403B-8D8C-6353D90F51FA}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -1174,23 +1173,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5DCA854-37C5-4AE6-A1F4-D8E5C19B7A23}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C4E48B-B382-41EB-A4E3-3450931EE1D5}">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A14"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1258,7 +1245,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD271BE-D4E3-4406-B763-12AFCA7F0CAC}">
   <dimension ref="A1:A11"/>
   <sheetViews>
@@ -1331,11 +1318,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C00ECEF-8F1B-4C1F-BC18-0B2C5C15443C}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>

</xml_diff>